<commit_message>
fixed instance variable bug on PE and UPE classes, untagged iface bug for Interface.tag value kudos to stackoverflow
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="4440" windowHeight="8565" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="4440" windowHeight="8565" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Devices" sheetId="1" r:id="rId1"/>
     <sheet name="Interfaces" sheetId="2" r:id="rId2"/>
+    <sheet name="L2ifaces" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="130">
   <si>
     <t>device</t>
   </si>
@@ -382,6 +383,39 @@
   </si>
   <si>
     <t>10.200.10.4</t>
+  </si>
+  <si>
+    <t>iface</t>
+  </si>
+  <si>
+    <t>descr</t>
+  </si>
+  <si>
+    <t>mode</t>
+  </si>
+  <si>
+    <t>allowed_vlans</t>
+  </si>
+  <si>
+    <t>trunk</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>ge1/10</t>
+  </si>
+  <si>
+    <t>gi1/48</t>
+  </si>
+  <si>
+    <t>10,20,30,110</t>
+  </si>
+  <si>
+    <t>40,50,60,110</t>
+  </si>
+  <si>
+    <t>70,80,90,200</t>
   </si>
 </sst>
 </file>
@@ -742,7 +776,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -981,8 +1015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1858,4 +1892,138 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" t="s">
+        <v>123</v>
+      </c>
+      <c r="E5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D6" t="s">
+        <v>123</v>
+      </c>
+      <c r="E6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updates on test data file; igp&vrf variations.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="4440" windowHeight="8565" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="4440" windowHeight="8565" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Devices" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="L2ifaces" sheetId="3" r:id="rId5"/>
     <sheet name="Vlans" sheetId="6" r:id="rId6"/>
     <sheet name="VRF" sheetId="5" r:id="rId7"/>
+    <sheet name="LIB" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="207">
   <si>
     <t>device</t>
   </si>
@@ -603,6 +604,54 @@
   </si>
   <si>
     <t>110,400,401,402</t>
+  </si>
+  <si>
+    <t>rd</t>
+  </si>
+  <si>
+    <t>10.224.0.1:100</t>
+  </si>
+  <si>
+    <t>10.224.0.2:100</t>
+  </si>
+  <si>
+    <t>10.224.0.3:100</t>
+  </si>
+  <si>
+    <t>10.224.0.4:100</t>
+  </si>
+  <si>
+    <t>65400:100</t>
+  </si>
+  <si>
+    <t>ipv4 import RT</t>
+  </si>
+  <si>
+    <t>ipv4 export RT</t>
+  </si>
+  <si>
+    <t>ipv6 import RT</t>
+  </si>
+  <si>
+    <t>ipv6 export RT</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Device</t>
+  </si>
+  <si>
+    <t>Interface</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>label proto</t>
+  </si>
+  <si>
+    <t>igp proto</t>
   </si>
 </sst>
 </file>
@@ -965,7 +1014,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1018,6 +1067,9 @@
       <c r="E2" t="s">
         <v>17</v>
       </c>
+      <c r="F2" t="s">
+        <v>49</v>
+      </c>
       <c r="G2" t="s">
         <v>36</v>
       </c>
@@ -1038,6 +1090,9 @@
       <c r="E3" t="s">
         <v>17</v>
       </c>
+      <c r="F3" t="s">
+        <v>2</v>
+      </c>
       <c r="G3" t="s">
         <v>36</v>
       </c>
@@ -1058,6 +1113,9 @@
       <c r="E4" t="s">
         <v>40</v>
       </c>
+      <c r="F4" t="s">
+        <v>49</v>
+      </c>
       <c r="G4" t="s">
         <v>37</v>
       </c>
@@ -1078,6 +1136,9 @@
       <c r="E5" t="s">
         <v>17</v>
       </c>
+      <c r="F5" t="s">
+        <v>2</v>
+      </c>
       <c r="G5" t="s">
         <v>37</v>
       </c>
@@ -1098,6 +1159,9 @@
       <c r="E6" t="s">
         <v>17</v>
       </c>
+      <c r="F6" t="s">
+        <v>3</v>
+      </c>
       <c r="G6" t="s">
         <v>37</v>
       </c>
@@ -1118,6 +1182,9 @@
       <c r="E7" t="s">
         <v>40</v>
       </c>
+      <c r="F7" t="s">
+        <v>4</v>
+      </c>
       <c r="G7" t="s">
         <v>37</v>
       </c>
@@ -1138,6 +1205,9 @@
       <c r="E8" t="s">
         <v>17</v>
       </c>
+      <c r="F8" t="s">
+        <v>5</v>
+      </c>
       <c r="G8" t="s">
         <v>38</v>
       </c>
@@ -1158,6 +1228,9 @@
       <c r="E9" t="s">
         <v>17</v>
       </c>
+      <c r="F9" t="s">
+        <v>6</v>
+      </c>
       <c r="G9" t="s">
         <v>38</v>
       </c>
@@ -1178,6 +1251,9 @@
       <c r="E10" t="s">
         <v>40</v>
       </c>
+      <c r="F10" t="s">
+        <v>7</v>
+      </c>
       <c r="G10" t="s">
         <v>39</v>
       </c>
@@ -1198,6 +1274,9 @@
       <c r="E11" t="s">
         <v>40</v>
       </c>
+      <c r="F11" t="s">
+        <v>8</v>
+      </c>
       <c r="G11" t="s">
         <v>39</v>
       </c>
@@ -1218,6 +1297,9 @@
       <c r="E12" t="s">
         <v>17</v>
       </c>
+      <c r="F12" t="s">
+        <v>27</v>
+      </c>
       <c r="G12" t="s">
         <v>36</v>
       </c>
@@ -1238,6 +1320,9 @@
       <c r="E13" t="s">
         <v>17</v>
       </c>
+      <c r="F13" t="s">
+        <v>28</v>
+      </c>
       <c r="G13" t="s">
         <v>36</v>
       </c>
@@ -1258,6 +1343,9 @@
       <c r="E14" t="s">
         <v>17</v>
       </c>
+      <c r="F14" t="s">
+        <v>29</v>
+      </c>
       <c r="G14" t="s">
         <v>37</v>
       </c>
@@ -1278,6 +1366,9 @@
       <c r="E15" t="s">
         <v>40</v>
       </c>
+      <c r="F15" t="s">
+        <v>50</v>
+      </c>
       <c r="G15" t="s">
         <v>36</v>
       </c>
@@ -1298,6 +1389,9 @@
       <c r="E16" t="s">
         <v>40</v>
       </c>
+      <c r="F16" t="s">
+        <v>48</v>
+      </c>
       <c r="G16" t="s">
         <v>36</v>
       </c>
@@ -1318,6 +1412,9 @@
       <c r="E17" t="s">
         <v>40</v>
       </c>
+      <c r="F17" t="s">
+        <v>51</v>
+      </c>
       <c r="G17" t="s">
         <v>36</v>
       </c>
@@ -1338,6 +1435,9 @@
       <c r="E18" t="s">
         <v>40</v>
       </c>
+      <c r="F18" t="s">
+        <v>52</v>
+      </c>
       <c r="G18" t="s">
         <v>36</v>
       </c>
@@ -1358,6 +1458,9 @@
       <c r="E19" t="s">
         <v>17</v>
       </c>
+      <c r="F19" t="s">
+        <v>56</v>
+      </c>
       <c r="G19" t="s">
         <v>37</v>
       </c>
@@ -1377,6 +1480,9 @@
       </c>
       <c r="E20" t="s">
         <v>17</v>
+      </c>
+      <c r="F20" t="s">
+        <v>57</v>
       </c>
       <c r="G20" t="s">
         <v>37</v>
@@ -2511,7 +2617,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
@@ -3154,14 +3260,172 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D4"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E1" t="s">
+        <v>198</v>
+      </c>
+      <c r="F1" t="s">
+        <v>199</v>
+      </c>
+      <c r="G1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E2" t="s">
+        <v>196</v>
+      </c>
+      <c r="F2" t="s">
+        <v>196</v>
+      </c>
+      <c r="G2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D3" t="s">
+        <v>196</v>
+      </c>
+      <c r="E3" t="s">
+        <v>196</v>
+      </c>
+      <c r="F3" t="s">
+        <v>196</v>
+      </c>
+      <c r="G3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4" t="s">
+        <v>201</v>
+      </c>
+      <c r="C4" t="s">
+        <v>194</v>
+      </c>
+      <c r="D4" t="s">
+        <v>196</v>
+      </c>
+      <c r="E4" t="s">
+        <v>196</v>
+      </c>
+      <c r="F4" t="s">
+        <v>196</v>
+      </c>
+      <c r="G4" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C5" t="s">
+        <v>195</v>
+      </c>
+      <c r="D5" t="s">
+        <v>196</v>
+      </c>
+      <c r="E5" t="s">
+        <v>196</v>
+      </c>
+      <c r="F5" t="s">
+        <v>196</v>
+      </c>
+      <c r="G5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
yet another commit. fixing jnpr templates
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -9,17 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="4440" windowHeight="8565" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="4440" windowHeight="8565" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Devices" sheetId="1" r:id="rId1"/>
     <sheet name="Interfaces" sheetId="2" r:id="rId2"/>
     <sheet name="AE" sheetId="7" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
-    <sheet name="L2ifaces" sheetId="3" r:id="rId5"/>
-    <sheet name="Vlans" sheetId="6" r:id="rId6"/>
-    <sheet name="VRF" sheetId="5" r:id="rId7"/>
-    <sheet name="LIB" sheetId="8" r:id="rId8"/>
+    <sheet name="L2ifaces" sheetId="3" r:id="rId4"/>
+    <sheet name="Vlans" sheetId="6" r:id="rId5"/>
+    <sheet name="VRF" sheetId="5" r:id="rId6"/>
+    <sheet name="LIB" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="215">
   <si>
     <t>device</t>
   </si>
@@ -652,6 +651,30 @@
   </si>
   <si>
     <t>igp proto</t>
+  </si>
+  <si>
+    <t>xe-11/0/0</t>
+  </si>
+  <si>
+    <t>Gi1/0/1</t>
+  </si>
+  <si>
+    <t>Gi1/0/2</t>
+  </si>
+  <si>
+    <t>Ten2/0/1</t>
+  </si>
+  <si>
+    <t>Ten2/0/2</t>
+  </si>
+  <si>
+    <t>Ten2/0/3</t>
+  </si>
+  <si>
+    <t>Ten2/0/4</t>
+  </si>
+  <si>
+    <t>loopback0</t>
   </si>
 </sst>
 </file>
@@ -1013,18 +1036,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1105,7 +1128,7 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>214</v>
       </c>
       <c r="D4" t="s">
         <v>49</v>
@@ -1174,7 +1197,7 @@
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>214</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
@@ -1243,7 +1266,7 @@
         <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>214</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
@@ -1266,7 +1289,7 @@
         <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>214</v>
       </c>
       <c r="D11" t="s">
         <v>8</v>
@@ -1358,7 +1381,7 @@
         <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>214</v>
       </c>
       <c r="D15" t="s">
         <v>50</v>
@@ -1381,7 +1404,7 @@
         <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>214</v>
       </c>
       <c r="D16" t="s">
         <v>48</v>
@@ -1404,7 +1427,7 @@
         <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>214</v>
       </c>
       <c r="D17" t="s">
         <v>51</v>
@@ -1427,7 +1450,7 @@
         <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>214</v>
       </c>
       <c r="D18" t="s">
         <v>52</v>
@@ -1497,8 +1520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1716,7 +1739,7 @@
         <v>60</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>210</v>
       </c>
       <c r="C7" t="s">
         <v>59</v>
@@ -1748,7 +1771,7 @@
         <v>60</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>211</v>
       </c>
       <c r="C8" t="s">
         <v>59</v>
@@ -1780,7 +1803,7 @@
         <v>60</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>212</v>
       </c>
       <c r="C9" t="s">
         <v>59</v>
@@ -1812,7 +1835,7 @@
         <v>60</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>213</v>
       </c>
       <c r="C10" t="s">
         <v>59</v>
@@ -2100,7 +2123,7 @@
         <v>157</v>
       </c>
       <c r="B19" t="s">
-        <v>78</v>
+        <v>108</v>
       </c>
       <c r="C19" t="s">
         <v>59</v>
@@ -2356,7 +2379,7 @@
         <v>53</v>
       </c>
       <c r="B27" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C27" t="s">
         <v>59</v>
@@ -2516,7 +2539,7 @@
         <v>159</v>
       </c>
       <c r="B32" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C32" t="s">
         <v>59</v>
@@ -2617,8 +2640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2643,7 +2666,7 @@
         <v>158</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>207</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -2654,7 +2677,7 @@
         <v>159</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>207</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -2665,7 +2688,7 @@
         <v>156</v>
       </c>
       <c r="B4" t="s">
-        <v>109</v>
+        <v>208</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -2676,7 +2699,7 @@
         <v>157</v>
       </c>
       <c r="B5" t="s">
-        <v>109</v>
+        <v>209</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -2687,7 +2710,7 @@
         <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>108</v>
+        <v>208</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -2698,7 +2721,7 @@
         <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>108</v>
+        <v>207</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -2709,7 +2732,7 @@
         <v>60</v>
       </c>
       <c r="B8" t="s">
-        <v>109</v>
+        <v>208</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -2720,7 +2743,7 @@
         <v>155</v>
       </c>
       <c r="B9" t="s">
-        <v>109</v>
+        <v>208</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -2731,7 +2754,7 @@
         <v>155</v>
       </c>
       <c r="B10" t="s">
-        <v>151</v>
+        <v>209</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -2742,7 +2765,7 @@
         <v>145</v>
       </c>
       <c r="B11" t="s">
-        <v>108</v>
+        <v>207</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -2753,7 +2776,7 @@
         <v>55</v>
       </c>
       <c r="B12" t="s">
-        <v>151</v>
+        <v>209</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -2764,7 +2787,7 @@
         <v>168</v>
       </c>
       <c r="B13" t="s">
-        <v>109</v>
+        <v>208</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -2775,7 +2798,7 @@
         <v>153</v>
       </c>
       <c r="B14" t="s">
-        <v>151</v>
+        <v>209</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -2786,7 +2809,7 @@
         <v>153</v>
       </c>
       <c r="B15" t="s">
-        <v>177</v>
+        <v>209</v>
       </c>
       <c r="C15">
         <v>4</v>
@@ -2797,7 +2820,7 @@
         <v>153</v>
       </c>
       <c r="B16" t="s">
-        <v>109</v>
+        <v>208</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -2808,7 +2831,7 @@
         <v>168</v>
       </c>
       <c r="B17" t="s">
-        <v>152</v>
+        <v>209</v>
       </c>
       <c r="C17">
         <v>3</v>
@@ -2819,7 +2842,7 @@
         <v>168</v>
       </c>
       <c r="B18" t="s">
-        <v>178</v>
+        <v>209</v>
       </c>
       <c r="C18">
         <v>5</v>
@@ -2830,7 +2853,10 @@
         <v>153</v>
       </c>
       <c r="B19" t="s">
-        <v>109</v>
+        <v>208</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2838,7 +2864,10 @@
         <v>168</v>
       </c>
       <c r="B20" t="s">
-        <v>109</v>
+        <v>208</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2846,7 +2875,10 @@
         <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>151</v>
+        <v>209</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2854,7 +2886,10 @@
         <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>152</v>
+        <v>209</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2862,7 +2897,10 @@
         <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>177</v>
+        <v>209</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2870,7 +2908,10 @@
         <v>42</v>
       </c>
       <c r="B24" t="s">
-        <v>178</v>
+        <v>209</v>
+      </c>
+      <c r="C24">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -2883,28 +2924,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.42578125" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
     <col min="5" max="5" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3169,7 +3199,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -3258,12 +3288,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F2" sqref="F2:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3395,11 +3425,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>

</xml_diff>